<commit_message>
Added RyanTest_Resume.xaml (required to upgrade uipath.system.activities to 22.4.1), added knowledgebase folder(skillsets.csv,jobfunc.csv,jobtitle.csv, new resumedata.csv
</commit_message>
<xml_diff>
--- a/input/Skillsets.xlsx
+++ b/input/Skillsets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\RACE\8 Team Project\Project_2 Job matches Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e6431dddeb4959f/Documents/UiPath/Diamond/sct9-diamond-proj2/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B2955B0-A840-4123-A8FE-164C7B0C0EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{3B2955B0-A840-4123-A8FE-164C7B0C0EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F95CC44-821C-4AA0-B00A-9451390A7649}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="390" windowWidth="20460" windowHeight="10740" xr2:uid="{EA6DF143-D2E1-4A81-8899-3A754AAD3F23}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{EA6DF143-D2E1-4A81-8899-3A754AAD3F23}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -676,483 +676,486 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB7974A-B1D0-4152-A0AF-E9FC210B88E6}">
   <dimension ref="A1:A95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
Added ResetResumesFolder for testing purposes; Still testing DocumentUnderstanding; Fixed Read/Get/Extract of wrong Job Ref
</commit_message>
<xml_diff>
--- a/input/Skillsets.xlsx
+++ b/input/Skillsets.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="410">
   <si>
     <t>Active Directory</t>
   </si>
@@ -478,9 +478,6 @@
   </si>
   <si>
     <t>Cashiering</t>
-  </si>
-  <si>
-    <t>Change</t>
   </si>
   <si>
     <t>Channel</t>
@@ -1621,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B410"/>
+  <dimension ref="A1:B409"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2102,12 +2099,12 @@
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>150</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>11</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
@@ -2137,42 +2134,42 @@
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>156</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>13</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
-        <v>157</v>
+      <c r="A92" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>14</v>
+        <v>157</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>158</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>16</v>
+        <v>158</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
@@ -2187,17 +2184,17 @@
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>161</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>18</v>
+        <v>161</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
@@ -2232,17 +2229,17 @@
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>168</v>
+        <v>19</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>20</v>
+        <v>168</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
@@ -2272,12 +2269,12 @@
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>174</v>
+        <v>21</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>21</v>
+        <v>174</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
@@ -2292,27 +2289,27 @@
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>177</v>
+        <v>22</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>22</v>
+        <v>177</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>178</v>
+        <v>23</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>24</v>
+        <v>178</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
@@ -2367,22 +2364,22 @@
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>189</v>
+        <v>25</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>25</v>
+        <v>189</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>190</v>
+        <v>26</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>26</v>
+        <v>190</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
@@ -2402,17 +2399,17 @@
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>194</v>
+        <v>27</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>28</v>
+        <v>194</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
@@ -2437,22 +2434,22 @@
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>199</v>
+        <v>29</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>29</v>
+        <v>199</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>200</v>
+        <v>30</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>30</v>
+        <v>200</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
@@ -2522,22 +2519,22 @@
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>214</v>
+        <v>31</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>31</v>
+        <v>214</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>215</v>
+        <v>32</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
@@ -2562,12 +2559,12 @@
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>220</v>
+        <v>34</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>34</v>
+        <v>220</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
@@ -2597,12 +2594,12 @@
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>226</v>
+        <v>36</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>36</v>
+        <v>226</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
@@ -2612,27 +2609,27 @@
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>228</v>
+        <v>37</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>37</v>
+        <v>228</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>229</v>
+        <v>38</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>39</v>
+        <v>229</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
@@ -2682,12 +2679,12 @@
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>239</v>
+        <v>40</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>40</v>
+        <v>239</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
@@ -2697,12 +2694,12 @@
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>241</v>
+        <v>41</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>41</v>
+        <v>241</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
@@ -2752,12 +2749,12 @@
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>251</v>
+        <v>42</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>42</v>
+        <v>251</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
@@ -2782,12 +2779,12 @@
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>256</v>
+        <v>44</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>44</v>
+        <v>256</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
@@ -2802,12 +2799,12 @@
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>259</v>
+        <v>45</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>45</v>
+        <v>259</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
@@ -2862,17 +2859,17 @@
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>270</v>
+        <v>46</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>47</v>
+        <v>270</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
@@ -2947,12 +2944,12 @@
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>285</v>
+        <v>48</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>48</v>
+        <v>285</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.3">
@@ -2972,12 +2969,12 @@
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>289</v>
+        <v>50</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>50</v>
+        <v>289</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.3">
@@ -3002,12 +2999,12 @@
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>294</v>
+        <v>51</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>51</v>
+        <v>294</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.3">
@@ -3037,27 +3034,27 @@
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>300</v>
+        <v>52</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>52</v>
+        <v>300</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>301</v>
+        <v>53</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>54</v>
+        <v>301</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.3">
@@ -3067,12 +3064,12 @@
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>303</v>
+        <v>55</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>55</v>
+        <v>303</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.3">
@@ -3102,12 +3099,12 @@
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>309</v>
+        <v>56</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>56</v>
+        <v>309</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.3">
@@ -3132,12 +3129,12 @@
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>314</v>
+        <v>57</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>57</v>
+        <v>314</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.3">
@@ -3147,12 +3144,12 @@
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>316</v>
+        <v>58</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>58</v>
+        <v>316</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.3">
@@ -3172,12 +3169,12 @@
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>320</v>
+        <v>60</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>60</v>
+        <v>320</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.3">
@@ -3207,12 +3204,12 @@
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>326</v>
+        <v>61</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>61</v>
+        <v>326</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.3">
@@ -3277,17 +3274,17 @@
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>339</v>
+        <v>62</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>63</v>
+        <v>339</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.3">
@@ -3307,17 +3304,17 @@
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>343</v>
+        <v>64</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>65</v>
+        <v>343</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.3">
@@ -3352,12 +3349,12 @@
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>350</v>
+        <v>66</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>66</v>
+        <v>350</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.3">
@@ -3407,22 +3404,22 @@
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>360</v>
+        <v>67</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>68</v>
+        <v>360</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.3">
@@ -3447,12 +3444,12 @@
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>365</v>
+        <v>69</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>69</v>
+        <v>365</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.3">
@@ -3462,12 +3459,12 @@
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>367</v>
+        <v>70</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>70</v>
+        <v>367</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.3">
@@ -3497,22 +3494,22 @@
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>373</v>
+        <v>71</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>73</v>
+        <v>373</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.3">
@@ -3542,12 +3539,12 @@
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>379</v>
+        <v>74</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
-        <v>74</v>
+        <v>379</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.3">
@@ -3557,12 +3554,12 @@
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>381</v>
+        <v>75</v>
       </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>75</v>
+        <v>381</v>
       </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.3">
@@ -3632,12 +3629,12 @@
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
-        <v>395</v>
+        <v>76</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
-        <v>76</v>
+        <v>395</v>
       </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.3">
@@ -3657,12 +3654,12 @@
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>399</v>
+        <v>77</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>77</v>
+        <v>399</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.3">
@@ -3677,22 +3674,22 @@
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
-        <v>402</v>
+        <v>79</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
-        <v>79</v>
+        <v>402</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
-        <v>403</v>
+        <v>80</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
-        <v>80</v>
+        <v>403</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.3">
@@ -3707,17 +3704,17 @@
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
-        <v>406</v>
+        <v>81</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
-        <v>82</v>
+        <v>406</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.3">
@@ -3727,22 +3724,17 @@
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
-        <v>408</v>
+        <v>83</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
-        <v>83</v>
+        <v>408</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>409</v>
-      </c>
-    </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A410" t="s">
-        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing GetRecommended7 to get all instead of just Recommended
</commit_message>
<xml_diff>
--- a/input/Skillsets.xlsx
+++ b/input/Skillsets.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\UiPath\SCT9_Diamond_Project2\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\UiPath\sct9-diamond-proj2 - Copy\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC618E25-ADEA-46D7-B429-5DFC7E458033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21816" windowHeight="14016"/>
+    <workbookView xWindow="340" yWindow="200" windowWidth="9280" windowHeight="10000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,22 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="462">
   <si>
     <t>Active Directory</t>
   </si>
@@ -1357,12 +1348,78 @@
   </si>
   <si>
     <t>Dot Net</t>
+  </si>
+  <si>
+    <t>Microsoft PowerPoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outsourcing </t>
+  </si>
+  <si>
+    <t>Investigation</t>
+  </si>
+  <si>
+    <t>MS Word</t>
+  </si>
+  <si>
+    <t>Microsoft Word</t>
+  </si>
+  <si>
+    <t>Able To Multitask</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Able To Work Independently</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document Management </t>
+  </si>
+  <si>
+    <t>Public Relations</t>
+  </si>
+  <si>
+    <t>Good Communication Skills</t>
+  </si>
+  <si>
+    <t>Communication Skills</t>
+  </si>
+  <si>
+    <t>Administrative Support</t>
+  </si>
+  <si>
+    <t>Circulation</t>
+  </si>
+  <si>
+    <t>Taxation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human Resources  </t>
+  </si>
+  <si>
+    <t>Employee Relations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continuous Improvement  </t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>Facility management</t>
+  </si>
+  <si>
+    <t>Document Controller</t>
+  </si>
+  <si>
+    <t>Shippings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1731,20 +1788,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B438"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B460"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <pane ySplit="1" topLeftCell="A443" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B452" sqref="B452"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
@@ -1752,842 +1809,842 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>33</v>
       </c>
@@ -2595,7 +2652,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>85</v>
       </c>
@@ -2603,7 +2660,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>86</v>
       </c>
@@ -2611,17 +2668,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>35</v>
       </c>
@@ -2629,7 +2686,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>87</v>
       </c>
@@ -2637,222 +2694,222 @@
         <v>35</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
         <v>43</v>
       </c>
@@ -2860,42 +2917,42 @@
         <v>45</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
         <v>89</v>
       </c>
@@ -2903,7 +2960,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
         <v>88</v>
       </c>
@@ -2911,167 +2968,167 @@
         <v>89</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" s="1" t="s">
         <v>90</v>
       </c>
@@ -3079,7 +3136,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" s="1" t="s">
         <v>49</v>
       </c>
@@ -3087,42 +3144,42 @@
         <v>90</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" s="1" t="s">
         <v>92</v>
       </c>
@@ -3130,7 +3187,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" s="1" t="s">
         <v>91</v>
       </c>
@@ -3138,167 +3195,167 @@
         <v>92</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A304" s="1" t="s">
         <v>93</v>
       </c>
@@ -3306,7 +3363,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A305" s="1" t="s">
         <v>59</v>
       </c>
@@ -3314,272 +3371,272 @@
         <v>93</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" s="1" t="s">
         <v>94</v>
       </c>
@@ -3587,157 +3644,157 @@
         <v>95</v>
       </c>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" s="1" t="s">
         <v>97</v>
       </c>
@@ -3745,27 +3802,27 @@
         <v>96</v>
       </c>
     </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" s="1" t="s">
         <v>96</v>
       </c>
@@ -3773,17 +3830,17 @@
         <v>97</v>
       </c>
     </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
         <v>415</v>
       </c>
@@ -3791,62 +3848,62 @@
         <v>435</v>
       </c>
     </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
         <v>435</v>
       </c>
@@ -3854,72 +3911,72 @@
         <v>415</v>
       </c>
     </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A424" s="1" t="s">
         <v>98</v>
       </c>
@@ -3927,12 +3984,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A426" s="1" t="s">
         <v>99</v>
       </c>
@@ -3940,69 +3997,179 @@
         <v>78</v>
       </c>
     </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
         <v>404</v>
       </c>
     </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A439" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A440" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A441" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A442" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A443" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A444" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A445" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A446" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A447" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A448" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A449" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A450" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A451" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A452" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A453" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A454" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A455" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A456" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A457" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A458" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A459" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A460" t="s">
+        <v>459</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B404">
-    <sortState ref="A2:B438">
+  <autoFilter ref="A1:B404" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B438">
       <sortCondition ref="A1:A404"/>
     </sortState>
   </autoFilter>

</xml_diff>